<commit_message>
feat: adding excel merge
</commit_message>
<xml_diff>
--- a/extract_list/outputs/benavides-suplementos.xlsx
+++ b/extract_list/outputs/benavides-suplementos.xlsx
@@ -1,108 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRUSS\Documents\web_scraping\proyecto_bra\finals\web-scraping-thomas\extract_details\outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>1037982</t>
-  </si>
-  <si>
-    <t>Nestlé MaterPlus Suplemento Alimenticio con DHA</t>
-  </si>
-  <si>
-    <t>30 Cápsulas</t>
-  </si>
-  <si>
-    <t>https://images.ctfassets.net/pcz6cf5u0j0b/Nncy5PQV3IR4tvlSWqe4D/239abb067e32afbdfffd4fc55b6140bb/7501058624017_MATERPLUS_DHA_34G_30CAP.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
-  </si>
-  <si>
-    <t>764388</t>
-  </si>
-  <si>
-    <t>Nestlé Materna Multivitamínico con Ácido Fólico</t>
-  </si>
-  <si>
-    <t>30 Tabletas</t>
-  </si>
-  <si>
-    <t>https://images.ctfassets.net/pcz6cf5u0j0b/3TqfvvzKZVO5xR15WBodEZ/1b78e2a0ee0917fd5f6ce35362928562/7501058625281_MATERNA_30TAB.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
-  </si>
-  <si>
-    <t>1038511</t>
-  </si>
-  <si>
-    <t>Ácido Fólico</t>
-  </si>
-  <si>
-    <t>0.4 mg — 180 Tabletas</t>
-  </si>
-  <si>
-    <t>https://images.ctfassets.net/pcz6cf5u0j0b/6vszAxH0qYCXYcnfK3eRa/2fbf7695c9686fe324b4058e8f4e605f/1038511_FABE_ACIDO_FOLICO_0.4MG_C180_TABS.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
-  </si>
-  <si>
-    <t>1039995</t>
-  </si>
-  <si>
-    <t>Vitamina C</t>
-  </si>
-  <si>
-    <t>60 Tabletas</t>
-  </si>
-  <si>
-    <t>https://images.ctfassets.net/pcz6cf5u0j0b/5cHaBExGiWupIRiaENPlac/10843f559b2a8c0494d72ba9db39eb81/1039995_FABE_VITAMINA_C_ADULTO_X60_TABS.PNG?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -441,90 +420,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="188.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1037982</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Nestlé MaterPlus Suplemento Alimenticio con DHA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>30 Cápsulas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/Nncy5PQV3IR4tvlSWqe4D/239abb067e32afbdfffd4fc55b6140bb/7501058624017_MATERPLUS_DHA_34G_30CAP.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>764388</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Nestlé Materna Multivitamínico con Ácido Fólico</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30 Tabletas</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/3TqfvvzKZVO5xR15WBodEZ/1b78e2a0ee0917fd5f6ce35362928562/7501058625281_MATERNA_30TAB.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1038511</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ácido Fólico</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.4 mg — 180 Tabletas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/6vszAxH0qYCXYcnfK3eRa/2fbf7695c9686fe324b4058e8f4e605f/1038511_FABE_ACIDO_FOLICO_0.4MG_C180_TABS.png?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1039995</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Vitamina C</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>60 Tabletas</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/5cHaBExGiWupIRiaENPlac/10843f559b2a8c0494d72ba9db39eb81/1039995_FABE_VITAMINA_C_ADULTO_X60_TABS.PNG?fit=pad&amp;f=center&amp;w=620&amp;fm=png&amp;fl=png8&amp;q=55</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Materna Nestlé MaterPlus Suplemento Alimenticio con DHA 30 Cápsulas | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/Nncy5PQV3IR4tvlSWqe4D/239abb067e32afbdfffd4fc55b6140bb/7501058624017_MATERPLUS_DHA_34G_30CAP.png?&amp;w=100&amp;h=100&amp;fit=pad&amp;fm=jpg&amp;fl=progressive&amp;q=25</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>36600</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Opti-Lac | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/6SXshvBKrBUQd4k103QMNU/7fdcd36b241cc1c50c8a6c480f07127b/7501058643049_NESTLE_OPTI-LAC_24X8.46G_MX.png?&amp;w=100&amp;h=100&amp;fit=pad&amp;fm=jpg&amp;fl=progressive&amp;q=25</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Materna Nestlé Materna Multivitamínico con Ácido Fólico 30 Tabletas | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/3TqfvvzKZVO5xR15WBodEZ/1b78e2a0ee0917fd5f6ce35362928562/7501058625281_MATERNA_30TAB.png?&amp;w=100&amp;h=100&amp;fit=pad&amp;fm=jpg&amp;fl=progressive&amp;q=25</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>24100</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Farmacias Benavides Vitamina C 60 Tabletas | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://images.ctfassets.net/pcz6cf5u0j0b/5cHaBExGiWupIRiaENPlac/10843f559b2a8c0494d72ba9db39eb81/1039995_FABE_VITAMINA_C_ADULTO_X60_TABS.PNG?&amp;w=100&amp;h=100&amp;fit=pad&amp;fm=jpg&amp;fl=progressive&amp;q=25</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9900</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Materna | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Baby &amp; Me | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Farmacias Benavides | Farmacias Benavides</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>